<commit_message>
Discover Applied Sciences - Revision-1
</commit_message>
<xml_diff>
--- a/Reviewer_Comments_R_1_19-Dec-2024.xlsx
+++ b/Reviewer_Comments_R_1_19-Dec-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\Publications\Article_Empirical_Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B63FF12-D218-4728-ADF8-17630A587747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72E3945-DF65-461D-802E-AB19029200BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="XXXX" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$1:$M$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$1:$O$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{2A6FEC64-4480-427D-8954-529C95993DC6}">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{2A6FEC64-4480-427D-8954-529C95993DC6}">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="173">
   <si>
     <t>Reviewer 1</t>
   </si>
@@ -1784,14 +1784,27 @@
 1) increase sample time, 2) reduce episode duration and 3) reduce size of mini-batch.
 One additional thing to try is to parallelize training. You can use Parallel Computing Toolbox for that, and to set this up, you pretty much need to set a flag in training options (see e.g. here).
 We are also working on adding more training algorithms for continuous action spaces that are more sample efficient, so I would check back when R2020a goes live.
-{Anderlini2019} - MATLAB suggestions</t>
+{Anderlini2019} - MATLAB suggestions
+{Yang2023ReducingTime} - JUST QUOTE!</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>LaTex</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Response</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2098,6 +2111,12 @@
       <name val="Cascadia Mono SemiBold"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -2377,7 +2396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2615,9 +2634,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2631,23 +2647,11 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -2761,48 +2765,73 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4037,11 +4066,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816F3457-95CC-4A5E-96D0-1EA42C9E78DF}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4050,45 +4079,52 @@
     <col min="2" max="2" width="2.140625" style="71" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.140625" style="62" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="85" customWidth="1"/>
-    <col min="6" max="6" width="64.140625" style="92" customWidth="1"/>
-    <col min="7" max="7" width="2.28515625" style="62" customWidth="1"/>
-    <col min="8" max="11" width="5.85546875" style="62" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="62" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="62" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="84" customWidth="1"/>
+    <col min="6" max="7" width="6.140625" style="84" customWidth="1"/>
+    <col min="8" max="8" width="60.5703125" style="148" customWidth="1"/>
+    <col min="9" max="9" width="2.28515625" style="62" customWidth="1"/>
+    <col min="10" max="13" width="5.85546875" style="62" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" style="62" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="62" customWidth="1"/>
+    <col min="16" max="16" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="72"/>
       <c r="B1" s="63"/>
       <c r="C1" s="9"/>
       <c r="D1" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="87" t="s">
+      <c r="E1" s="140" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="140" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" s="140" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="141" t="s">
         <v>135</v>
       </c>
-      <c r="G1" s="93"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="116" t="s">
+      <c r="I1" s="88"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="111" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="116" t="s">
+      <c r="L1" s="111" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="116" t="s">
+      <c r="M1" s="111" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="117" t="s">
+      <c r="N1" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="M1" s="93"/>
-    </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="88"/>
+    </row>
+    <row r="2" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="73" t="s">
         <v>105</v>
       </c>
@@ -4101,29 +4137,33 @@
       <c r="D2" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="111" t="s">
+      <c r="E2" s="106" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="88"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="98" t="s">
+      <c r="F2" s="106" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="61"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="93" t="s">
         <v>129</v>
       </c>
-      <c r="I2" s="118">
+      <c r="K2" s="113">
         <f>COUNTA(C2)</f>
         <v>1</v>
       </c>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118">
+      <c r="L2" s="113"/>
+      <c r="M2" s="113">
         <v>1</v>
       </c>
-      <c r="L2" s="119">
-        <f>I2-K2</f>
+      <c r="N2" s="114">
+        <f>K2-M2</f>
         <v>0</v>
       </c>
-      <c r="M2" s="94"/>
-    </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="89"/>
+    </row>
+    <row r="3" spans="1:15" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
         <v>23</v>
       </c>
@@ -4136,29 +4176,31 @@
       <c r="D3" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="89"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="99" t="s">
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="118">
+      <c r="K3" s="113">
         <f>COUNTA(C3:C11)</f>
         <v>9</v>
       </c>
-      <c r="J3" s="118">
+      <c r="L3" s="113">
         <v>3</v>
       </c>
-      <c r="K3" s="118"/>
-      <c r="L3" s="119">
-        <f t="shared" ref="L3:L5" si="0">I3-K3</f>
+      <c r="M3" s="113"/>
+      <c r="N3" s="114">
+        <f t="shared" ref="N3:N5" si="0">K3-M3</f>
         <v>9</v>
       </c>
-      <c r="M3" s="94"/>
-    </row>
-    <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="89"/>
+    </row>
+    <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
         <v>23</v>
       </c>
@@ -4171,33 +4213,35 @@
       <c r="D4" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="113" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="89" t="s">
+      <c r="E4" s="102" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="143" t="s">
         <v>166</v>
       </c>
-      <c r="G4" s="94"/>
-      <c r="H4" s="100" t="s">
+      <c r="I4" s="89"/>
+      <c r="J4" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="120">
+      <c r="K4" s="115">
         <f>COUNTA(C12:C23)</f>
         <v>12</v>
       </c>
-      <c r="J4" s="120">
+      <c r="L4" s="115">
         <v>1</v>
       </c>
-      <c r="K4" s="120">
+      <c r="M4" s="115">
         <v>1</v>
       </c>
-      <c r="L4" s="121">
+      <c r="N4" s="116">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M4" s="94"/>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O4" s="89"/>
+    </row>
+    <row r="5" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="74"/>
       <c r="B5" s="66">
         <v>2</v>
@@ -4208,32 +4252,34 @@
       <c r="D5" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="95" t="s">
+      <c r="E5" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="89" t="s">
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="143" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="94"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="122">
-        <f>SUM(I2:I4)</f>
+      <c r="I5" s="89"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="117">
+        <f>SUM(K2:K4)</f>
         <v>22</v>
       </c>
-      <c r="J5" s="122">
-        <f>SUM(J2:J4)</f>
+      <c r="L5" s="117">
+        <f>SUM(L2:L4)</f>
         <v>4</v>
       </c>
-      <c r="K5" s="122">
+      <c r="M5" s="117">
         <v>2</v>
       </c>
-      <c r="L5" s="123">
+      <c r="N5" s="118">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="M5" s="94"/>
-    </row>
-    <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="89"/>
+    </row>
+    <row r="6" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
         <v>23</v>
       </c>
@@ -4246,30 +4292,32 @@
       <c r="D6" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="82" t="s">
+      <c r="E6" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="89" t="s">
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="143" t="s">
         <v>155</v>
       </c>
-      <c r="G6" s="94"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="94"/>
-      <c r="J6" s="124">
-        <f>J5/$I$5</f>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="119">
+        <f>L5/$K$5</f>
         <v>0.18181818181818182</v>
       </c>
-      <c r="K6" s="124">
-        <f>K5/$I$5</f>
+      <c r="M6" s="119">
+        <f>M5/$K$5</f>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="L6" s="124">
-        <f>L5/$I$5</f>
+      <c r="N6" s="119">
+        <f>N5/$K$5</f>
         <v>0.90909090909090906</v>
       </c>
-      <c r="M6" s="94"/>
-    </row>
-    <row r="7" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="89"/>
+    </row>
+    <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
         <v>23</v>
       </c>
@@ -4282,23 +4330,25 @@
       <c r="D7" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="E7" s="82" t="s">
+      <c r="E7" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="89"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="114" t="s">
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="143"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="109" t="s">
         <v>131</v>
       </c>
-      <c r="I7" s="129">
-        <v>45653</v>
-      </c>
-      <c r="J7" s="129"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
-    </row>
-    <row r="8" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="124">
+        <v>45657</v>
+      </c>
+      <c r="L7" s="124"/>
+      <c r="M7" s="89"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="89"/>
+    </row>
+    <row r="8" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
         <v>23</v>
       </c>
@@ -4311,24 +4361,26 @@
       <c r="D8" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="89"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="114" t="s">
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="143"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="109" t="s">
         <v>132</v>
       </c>
-      <c r="I8" s="129">
+      <c r="K8" s="124">
         <f ca="1">TODAY()</f>
         <v>45648</v>
       </c>
-      <c r="J8" s="129"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-    </row>
-    <row r="9" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="124"/>
+      <c r="M8" s="89"/>
+      <c r="N8" s="89"/>
+      <c r="O8" s="89"/>
+    </row>
+    <row r="9" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="74"/>
       <c r="B9" s="66">
         <v>5</v>
@@ -4339,26 +4391,28 @@
       <c r="D9" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="E9" s="113" t="s">
+      <c r="E9" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="89" t="s">
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="143" t="s">
         <v>153</v>
       </c>
-      <c r="G9" s="94"/>
-      <c r="H9" s="114" t="s">
+      <c r="I9" s="89"/>
+      <c r="J9" s="109" t="s">
         <v>96</v>
       </c>
-      <c r="I9" s="94">
-        <f ca="1">I7-I8-1</f>
-        <v>4</v>
-      </c>
-      <c r="J9" s="115"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-    </row>
-    <row r="10" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="89">
+        <f ca="1">K7-K8-1</f>
+        <v>8</v>
+      </c>
+      <c r="L9" s="110"/>
+      <c r="M9" s="89"/>
+      <c r="N9" s="89"/>
+      <c r="O9" s="89"/>
+    </row>
+    <row r="10" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
         <v>23</v>
       </c>
@@ -4371,21 +4425,23 @@
       <c r="D10" s="78" t="s">
         <v>111</v>
       </c>
-      <c r="E10" s="113" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="101" t="s">
+      <c r="E10" s="102" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="144" t="s">
         <v>154</v>
       </c>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="94"/>
-      <c r="L10" s="94"/>
-      <c r="M10" s="94"/>
-    </row>
-    <row r="11" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
+    </row>
+    <row r="11" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="75"/>
       <c r="B11" s="68">
         <v>6</v>
@@ -4396,19 +4452,21 @@
       <c r="D11" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="E11" s="83" t="s">
+      <c r="E11" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="90"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
-      <c r="M11" s="94"/>
-    </row>
-    <row r="12" spans="1:13" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="145"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="89"/>
+      <c r="O11" s="89"/>
+    </row>
+    <row r="12" spans="1:15" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
         <v>59</v>
       </c>
@@ -4421,19 +4479,21 @@
       <c r="D12" s="78" t="s">
         <v>113</v>
       </c>
-      <c r="E12" s="82" t="s">
+      <c r="E12" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="89"/>
-      <c r="G12" s="94"/>
-      <c r="H12" s="94"/>
-      <c r="I12" s="94"/>
-      <c r="J12" s="94"/>
-      <c r="K12" s="94"/>
-      <c r="L12" s="94"/>
-      <c r="M12" s="94"/>
-    </row>
-    <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="143"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
+    </row>
+    <row r="13" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
         <v>59</v>
       </c>
@@ -4446,19 +4506,21 @@
       <c r="D13" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="E13" s="82" t="s">
+      <c r="E13" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="F13" s="89"/>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="94"/>
-    </row>
-    <row r="14" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="143"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
+    </row>
+    <row r="14" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="74"/>
       <c r="B14" s="66">
         <v>2</v>
@@ -4469,19 +4531,21 @@
       <c r="D14" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="82" t="s">
+      <c r="E14" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="89"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
-      <c r="K14" s="94"/>
-      <c r="L14" s="94"/>
-      <c r="M14" s="94"/>
-    </row>
-    <row r="15" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="143"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="89"/>
+      <c r="O14" s="89"/>
+    </row>
+    <row r="15" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="74"/>
       <c r="B15" s="66">
         <v>2</v>
@@ -4492,19 +4556,21 @@
       <c r="D15" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="82" t="s">
+      <c r="E15" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="F15" s="89"/>
-      <c r="G15" s="94"/>
-      <c r="H15" s="94"/>
-      <c r="I15" s="94"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-    </row>
-    <row r="16" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="143"/>
+      <c r="I15" s="89"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="89"/>
+      <c r="L15" s="89"/>
+      <c r="M15" s="89"/>
+      <c r="N15" s="89"/>
+      <c r="O15" s="89"/>
+    </row>
+    <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
         <v>59</v>
       </c>
@@ -4517,19 +4583,21 @@
       <c r="D16" s="78" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="82" t="s">
+      <c r="E16" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="89"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="94"/>
-      <c r="I16" s="94"/>
-      <c r="J16" s="94"/>
-      <c r="K16" s="94"/>
-      <c r="L16" s="94"/>
-      <c r="M16" s="94"/>
-    </row>
-    <row r="17" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="143"/>
+      <c r="I16" s="89"/>
+      <c r="J16" s="89"/>
+      <c r="K16" s="89"/>
+      <c r="L16" s="89"/>
+      <c r="M16" s="89"/>
+      <c r="N16" s="89"/>
+      <c r="O16" s="89"/>
+    </row>
+    <row r="17" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
         <v>59</v>
       </c>
@@ -4542,21 +4610,23 @@
       <c r="D17" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="E17" s="82" t="s">
+      <c r="E17" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="86" t="s">
+      <c r="F17" s="85"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="146" t="s">
         <v>128</v>
       </c>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="94"/>
-      <c r="J17" s="94"/>
-      <c r="K17" s="94"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="94"/>
-    </row>
-    <row r="18" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="89"/>
+    </row>
+    <row r="18" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
         <v>59</v>
       </c>
@@ -4569,21 +4639,23 @@
       <c r="D18" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="113" t="s">
+      <c r="E18" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="89" t="s">
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="143" t="s">
         <v>152</v>
       </c>
-      <c r="G18" s="94"/>
-      <c r="H18" s="94"/>
-      <c r="I18" s="94"/>
-      <c r="J18" s="94"/>
-      <c r="K18" s="94"/>
-      <c r="L18" s="94"/>
-      <c r="M18" s="94"/>
-    </row>
-    <row r="19" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="89"/>
+      <c r="M18" s="89"/>
+      <c r="N18" s="89"/>
+      <c r="O18" s="89"/>
+    </row>
+    <row r="19" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
         <v>59</v>
       </c>
@@ -4596,19 +4668,21 @@
       <c r="D19" s="78" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="82" t="s">
+      <c r="E19" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="F19" s="89"/>
-      <c r="G19" s="94"/>
-      <c r="H19" s="94"/>
-      <c r="I19" s="94"/>
-      <c r="J19" s="94"/>
-      <c r="K19" s="94"/>
-      <c r="L19" s="94"/>
-      <c r="M19" s="94"/>
-    </row>
-    <row r="20" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="143"/>
+      <c r="I19" s="89"/>
+      <c r="J19" s="89"/>
+      <c r="K19" s="89"/>
+      <c r="L19" s="89"/>
+      <c r="M19" s="89"/>
+      <c r="N19" s="89"/>
+      <c r="O19" s="89"/>
+    </row>
+    <row r="20" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="74" t="s">
         <v>59</v>
       </c>
@@ -4621,19 +4695,21 @@
       <c r="D20" s="78" t="s">
         <v>120</v>
       </c>
-      <c r="E20" s="82" t="s">
+      <c r="E20" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="F20" s="89"/>
-      <c r="G20" s="94"/>
-      <c r="H20" s="94"/>
-      <c r="I20" s="94"/>
-      <c r="J20" s="94"/>
-      <c r="K20" s="94"/>
-      <c r="L20" s="94"/>
-      <c r="M20" s="94"/>
-    </row>
-    <row r="21" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="143"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="89"/>
+      <c r="K20" s="89"/>
+      <c r="L20" s="89"/>
+      <c r="M20" s="89"/>
+      <c r="N20" s="89"/>
+      <c r="O20" s="89"/>
+    </row>
+    <row r="21" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="74"/>
       <c r="B21" s="66">
         <v>7</v>
@@ -4644,21 +4720,25 @@
       <c r="D21" s="78" t="s">
         <v>121</v>
       </c>
-      <c r="E21" s="107" t="s">
+      <c r="E21" s="102" t="s">
         <v>130</v>
       </c>
-      <c r="F21" s="89" t="s">
+      <c r="F21" s="86" t="s">
+        <v>171</v>
+      </c>
+      <c r="G21" s="86"/>
+      <c r="H21" s="143" t="s">
         <v>137</v>
       </c>
-      <c r="G21" s="94"/>
-      <c r="H21" s="94"/>
-      <c r="I21" s="94"/>
-      <c r="J21" s="94"/>
-      <c r="K21" s="94"/>
-      <c r="L21" s="94"/>
-      <c r="M21" s="94"/>
-    </row>
-    <row r="22" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="89"/>
+      <c r="J21" s="89"/>
+      <c r="K21" s="89"/>
+      <c r="L21" s="89"/>
+      <c r="M21" s="89"/>
+      <c r="N21" s="89"/>
+      <c r="O21" s="89"/>
+    </row>
+    <row r="22" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="74" t="s">
         <v>59</v>
       </c>
@@ -4671,19 +4751,21 @@
       <c r="D22" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="E22" s="82" t="s">
+      <c r="E22" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="F22" s="89"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="94"/>
-      <c r="I22" s="94"/>
-      <c r="J22" s="94"/>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-    </row>
-    <row r="23" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="143"/>
+      <c r="I22" s="89"/>
+      <c r="J22" s="89"/>
+      <c r="K22" s="89"/>
+      <c r="L22" s="89"/>
+      <c r="M22" s="89"/>
+      <c r="N22" s="89"/>
+      <c r="O22" s="89"/>
+    </row>
+    <row r="23" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="75" t="s">
         <v>59</v>
       </c>
@@ -4696,42 +4778,46 @@
       <c r="D23" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="83" t="s">
+      <c r="E23" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="90"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="94"/>
-      <c r="I23" s="94"/>
-      <c r="J23" s="94"/>
-      <c r="K23" s="94"/>
-      <c r="L23" s="94"/>
-      <c r="M23" s="94"/>
-    </row>
-    <row r="24" spans="1:13" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="145"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="89"/>
+      <c r="L23" s="89"/>
+      <c r="M23" s="89"/>
+      <c r="N23" s="89"/>
+      <c r="O23" s="89"/>
+    </row>
+    <row r="24" spans="1:15" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="76"/>
       <c r="B24" s="70"/>
       <c r="C24" s="32"/>
       <c r="D24" s="80"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="91"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="94"/>
-      <c r="J24" s="94"/>
-      <c r="K24" s="94"/>
-      <c r="L24" s="94"/>
-      <c r="M24" s="94"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="147"/>
+      <c r="I24" s="89"/>
+      <c r="J24" s="89"/>
+      <c r="L24" s="89"/>
+      <c r="M24" s="89"/>
+      <c r="N24" s="89"/>
+      <c r="O24" s="89"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M23" xr:uid="{816F3457-95CC-4A5E-96D0-1EA42C9E78DF}"/>
+  <autoFilter ref="A1:O23" xr:uid="{816F3457-95CC-4A5E-96D0-1EA42C9E78DF}"/>
   <mergeCells count="2">
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I3:I4" formulaRange="1"/>
+    <ignoredError sqref="K3:K4" formulaRange="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -4742,53 +4828,53 @@
   <dimension ref="B2:G27"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" style="104" customWidth="1"/>
-    <col min="3" max="3" width="98.7109375" style="104" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="99" customWidth="1"/>
+    <col min="3" max="3" width="98.7109375" style="99" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="121" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="126"/>
+      <c r="C2" s="121"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="97" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="C4" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="98" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D5" s="104"/>
+      <c r="D5" s="99"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="102" t="s">
+      <c r="B6" s="97" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="112" t="s">
+      <c r="D6" s="107" t="s">
         <v>150</v>
       </c>
-      <c r="E6" s="112" t="s">
+      <c r="E6" s="107" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="104" t="s">
+      <c r="C7" s="99" t="s">
         <v>144</v>
       </c>
       <c r="D7">
@@ -4799,7 +4885,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="104" t="s">
+      <c r="C8" s="99" t="s">
         <v>146</v>
       </c>
       <c r="D8">
@@ -4810,7 +4896,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="104" t="s">
+      <c r="C9" s="99" t="s">
         <v>149</v>
       </c>
       <c r="D9">
@@ -4821,7 +4907,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="106" t="s">
+      <c r="B10" s="101" t="s">
         <v>148</v>
       </c>
       <c r="D10">
@@ -4832,7 +4918,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="105" t="s">
+      <c r="C11" s="100" t="s">
         <v>147</v>
       </c>
       <c r="D11">
@@ -4843,10 +4929,10 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="102" t="s">
+      <c r="B12" s="97" t="s">
         <v>143</v>
       </c>
-      <c r="C12" s="125" t="s">
+      <c r="C12" s="120" t="s">
         <v>156</v>
       </c>
       <c r="D12">
@@ -4857,49 +4943,49 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="100" t="s">
         <v>162</v>
       </c>
-      <c r="C13" s="105" t="s">
+      <c r="C13" s="100" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="99" t="s">
         <v>163</v>
       </c>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="100" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="128" t="s">
+      <c r="B15" s="123" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="127" t="s">
+      <c r="C15" s="122" t="s">
         <v>159</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="78"/>
     </row>
     <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B17" s="125" t="s">
+      <c r="B17" s="120" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="105" t="s">
+      <c r="C17" s="100" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="B19" s="102" t="s">
+    <row r="19" spans="2:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="B19" s="97" t="s">
         <v>167</v>
       </c>
-      <c r="C19" s="105" t="s">
+      <c r="C19" s="100" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="105"/>
+      <c r="C20" s="100"/>
       <c r="F20" s="66">
         <v>2</v>
       </c>
@@ -4908,10 +4994,10 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="101" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="105" t="s">
+      <c r="C27" s="100" t="s">
         <v>139</v>
       </c>
     </row>
@@ -5435,12 +5521,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="103" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="104" t="s">
         <v>140</v>
       </c>
     </row>
@@ -5649,7 +5735,7 @@
       <c r="B3" s="41">
         <v>1</v>
       </c>
-      <c r="C3" s="110" t="s">
+      <c r="C3" s="105" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="44" t="s">
@@ -6180,19 +6266,19 @@
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="130" t="s">
+      <c r="A7" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="132">
+      <c r="B7" s="127">
         <v>1</v>
       </c>
-      <c r="C7" s="134" t="s">
+      <c r="C7" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="136" t="s">
+      <c r="D7" s="131" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="138" t="s">
+      <c r="E7" s="133" t="s">
         <v>38</v>
       </c>
       <c r="F7" s="26" t="s">
@@ -6200,11 +6286,11 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="140"/>
-      <c r="B8" s="141"/>
-      <c r="C8" s="142"/>
-      <c r="D8" s="143"/>
-      <c r="E8" s="144"/>
+      <c r="A8" s="126"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="130"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="134"/>
       <c r="F8" s="27" t="s">
         <v>40</v>
       </c>
@@ -6230,19 +6316,19 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="130" t="s">
+      <c r="A10" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="132">
+      <c r="B10" s="127">
         <v>3</v>
       </c>
-      <c r="C10" s="134" t="s">
+      <c r="C10" s="129" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="136" t="s">
+      <c r="D10" s="131" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="136" t="s">
+      <c r="E10" s="131" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="26" t="s">
@@ -6250,29 +6336,29 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="140"/>
-      <c r="B11" s="141"/>
-      <c r="C11" s="142"/>
-      <c r="D11" s="143"/>
-      <c r="E11" s="143"/>
+      <c r="A11" s="126"/>
+      <c r="B11" s="128"/>
+      <c r="C11" s="130"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="132"/>
       <c r="F11" s="21" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="130" t="s">
+      <c r="A12" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="132">
+      <c r="B12" s="127">
         <v>4</v>
       </c>
-      <c r="C12" s="134" t="s">
+      <c r="C12" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="136" t="s">
+      <c r="D12" s="131" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="136" t="s">
+      <c r="E12" s="131" t="s">
         <v>49</v>
       </c>
       <c r="F12" s="26" t="s">
@@ -6280,29 +6366,29 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="140"/>
-      <c r="B13" s="141"/>
-      <c r="C13" s="142"/>
-      <c r="D13" s="143"/>
-      <c r="E13" s="143"/>
+      <c r="A13" s="126"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="132"/>
       <c r="F13" s="21" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="130" t="s">
+      <c r="A14" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="132">
+      <c r="B14" s="127">
         <v>5</v>
       </c>
-      <c r="C14" s="134" t="s">
+      <c r="C14" s="129" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="136" t="s">
+      <c r="D14" s="131" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="136" t="s">
+      <c r="E14" s="131" t="s">
         <v>53</v>
       </c>
       <c r="F14" s="26" t="s">
@@ -6310,29 +6396,29 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="140"/>
-      <c r="B15" s="141"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="143"/>
-      <c r="E15" s="143"/>
+      <c r="A15" s="126"/>
+      <c r="B15" s="128"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="132"/>
       <c r="F15" s="27" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="130" t="s">
+      <c r="A16" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="132">
+      <c r="B16" s="127">
         <v>6</v>
       </c>
-      <c r="C16" s="134" t="s">
+      <c r="C16" s="129" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="136" t="s">
+      <c r="D16" s="131" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="138" t="s">
+      <c r="E16" s="133" t="s">
         <v>38</v>
       </c>
       <c r="F16" s="30" t="s">
@@ -6340,10 +6426,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="131"/>
-      <c r="B17" s="133"/>
-      <c r="C17" s="135"/>
-      <c r="D17" s="137"/>
+      <c r="A17" s="135"/>
+      <c r="B17" s="136"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="138"/>
       <c r="E17" s="139"/>
       <c r="F17" s="31" t="s">
         <v>58</v>
@@ -6584,31 +6670,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>